<commit_message>
Generalized BFIAF to FFIAF
Generated BFIAF Images and VFIAF Images
</commit_message>
<xml_diff>
--- a/xl_data/otero-bfiaf-CENSORED.xlsx
+++ b/xl_data/otero-bfiaf-CENSORED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\damon\COFC\bad-author\xl_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4833E21-7B32-43E9-945F-4339BE9CAE20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EEBFBD-66A6-4625-ADB9-98F5395E9A2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phpmyadmin" sheetId="1" r:id="rId1"/>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1298,7 +1298,7 @@
         <v>2.3219280948873622</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="25" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="10">
         <f>SUM(B2:B14)</f>
@@ -1508,7 +1508,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:O16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1517,6 +1517,7 @@
     <col min="2" max="2" width="7.90625" customWidth="1"/>
     <col min="4" max="4" width="9.08984375" customWidth="1"/>
     <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="15" max="15" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2236,7 +2237,7 @@
         <v>11.11196210668224</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" ht="25" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="10">
         <f>SUM(B2:B15)</f>
@@ -2463,8 +2464,8 @@
   </sheetPr>
   <dimension ref="A1:AS36"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A36" sqref="A1:AS36"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7300,83 +7301,83 @@
         <v>11.720671786825557</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" ht="37" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="10">
-        <f>SUM(B23:B35)</f>
-        <v>0</v>
+        <f>SUM(B2:B35)</f>
+        <v>32.883674585560556</v>
       </c>
       <c r="C36" s="10">
-        <f t="shared" ref="C36:AR36" si="1">SUM(C23:C35)</f>
-        <v>0</v>
+        <f t="shared" ref="C36:AR36" si="1">SUM(C2:C35)</f>
+        <v>4.7548875021634691</v>
       </c>
       <c r="D36" s="10">
         <f t="shared" si="1"/>
-        <v>14.068905956085185</v>
+        <v>66.806146960012626</v>
       </c>
       <c r="E36" s="10">
         <f t="shared" si="1"/>
-        <v>82.044702507778894</v>
+        <v>106.48767418208662</v>
       </c>
       <c r="F36" s="10">
         <f t="shared" si="1"/>
-        <v>4.8137811912170374</v>
+        <v>10.65998386012645</v>
       </c>
       <c r="G36" s="10">
         <f t="shared" si="1"/>
-        <v>6.7206717868255561</v>
+        <v>78.178469338230343</v>
       </c>
       <c r="H36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10.568668693380507</v>
       </c>
       <c r="I36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.253166867652578</v>
       </c>
       <c r="J36" s="10">
         <f t="shared" si="1"/>
-        <v>3.8137811912170374</v>
+        <v>9.8905967882678691</v>
       </c>
       <c r="K36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>18.835858127899954</v>
       </c>
       <c r="L36" s="10">
         <f t="shared" si="1"/>
-        <v>17.840087265589304</v>
+        <v>53.774713932316708</v>
       </c>
       <c r="M36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.032421477692377</v>
       </c>
       <c r="N36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>3.8137811912170374</v>
       </c>
       <c r="O36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>39.422750839558972</v>
       </c>
       <c r="P36" s="10">
         <f t="shared" si="1"/>
-        <v>5.4413435736511104</v>
+        <v>7.7632716685384722</v>
       </c>
       <c r="Q36" s="10">
         <f t="shared" si="1"/>
-        <v>11.627562382434077</v>
+        <v>24.583002126086701</v>
       </c>
       <c r="R36" s="10">
         <f t="shared" si="1"/>
-        <v>2.9068905956085191</v>
+        <v>13.24494636084761</v>
       </c>
       <c r="S36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>5.2612401681882579</v>
       </c>
       <c r="T36" s="10">
         <f t="shared" si="1"/>
-        <v>3.9068905956085191</v>
+        <v>7.3987436919381944</v>
       </c>
       <c r="U36" s="10">
         <f t="shared" si="1"/>
@@ -7388,11 +7389,11 @@
       </c>
       <c r="W36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9068905956085189</v>
       </c>
       <c r="X36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>2.9393120733008953</v>
       </c>
       <c r="Y36" s="10">
         <f t="shared" si="1"/>
@@ -7400,15 +7401,15 @@
       </c>
       <c r="Z36" s="10">
         <f t="shared" si="1"/>
-        <v>2.9068905956085191</v>
+        <v>5.5913887698805897</v>
       </c>
       <c r="AA36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>11.601090171072883</v>
       </c>
       <c r="AB36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.4918530963296752</v>
       </c>
       <c r="AC36" s="10">
         <f t="shared" si="1"/>
@@ -7416,11 +7417,11 @@
       </c>
       <c r="AD36" s="10">
         <f t="shared" si="1"/>
-        <v>3.8137811912170374</v>
+        <v>5.720671786825557</v>
       </c>
       <c r="AE36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>6.8462026689094149</v>
       </c>
       <c r="AF36" s="10">
         <f t="shared" si="1"/>
@@ -7428,31 +7429,31 @@
       </c>
       <c r="AG36" s="10">
         <f t="shared" si="1"/>
-        <v>26.653868456806347</v>
+        <v>253.88607621637183</v>
       </c>
       <c r="AH36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.684498174272071</v>
       </c>
       <c r="AI36" s="10">
         <f t="shared" si="1"/>
-        <v>12.627562382434075</v>
+        <v>14.659983860126452</v>
       </c>
       <c r="AJ36" s="10">
         <f t="shared" si="1"/>
-        <v>3.9068905956085191</v>
+        <v>29.924646366616862</v>
       </c>
       <c r="AK36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.169925001442313</v>
       </c>
       <c r="AL36" s="10">
         <f t="shared" si="1"/>
-        <v>2.9068905956085191</v>
+        <v>4.8137811912170383</v>
       </c>
       <c r="AM36" s="10">
         <f t="shared" si="1"/>
-        <v>0.90689059560851848</v>
+        <v>2.9393120733008953</v>
       </c>
       <c r="AN36" s="10">
         <f t="shared" si="1"/>
@@ -7460,19 +7461,19 @@
       </c>
       <c r="AO36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9068905956085189</v>
       </c>
       <c r="AP36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9068905956085189</v>
       </c>
       <c r="AQ36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5849625007211561</v>
       </c>
       <c r="AR36" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5849625007211561</v>
       </c>
       <c r="AS36" s="6"/>
     </row>

</xml_diff>